<commit_message>
Added output for tables I, III, IV.
</commit_message>
<xml_diff>
--- a/output/table_I.xlsx
+++ b/output/table_I.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>i</t>
   </si>
@@ -20,52 +20,64 @@
     <t>t</t>
   </si>
   <si>
-    <t>coef1_ols</t>
-  </si>
-  <si>
-    <t>coef2_ols</t>
-  </si>
-  <si>
-    <t>sd1_ols</t>
-  </si>
-  <si>
-    <t>sd2_ols</t>
-  </si>
-  <si>
-    <t>coef1_within</t>
-  </si>
-  <si>
-    <t>coef2_within</t>
-  </si>
-  <si>
-    <t>sd1_within</t>
-  </si>
-  <si>
-    <t>sd2_within</t>
-  </si>
-  <si>
     <t>coef1_infeasible</t>
   </si>
   <si>
     <t>coef2_infeasible</t>
   </si>
   <si>
+    <t>coef3_infeasible</t>
+  </si>
+  <si>
+    <t>coef4_infeasible</t>
+  </si>
+  <si>
+    <t>coef5_infeasible</t>
+  </si>
+  <si>
     <t>sd1_infeasible</t>
   </si>
   <si>
     <t>sd2_infeasible</t>
   </si>
   <si>
+    <t>sd3_infeasible</t>
+  </si>
+  <si>
+    <t>sd4_infeasible</t>
+  </si>
+  <si>
+    <t>sd5_infeasible</t>
+  </si>
+  <si>
     <t>coef1_interactive</t>
   </si>
   <si>
     <t>coef2_interactive</t>
   </si>
   <si>
+    <t>coef3_interactive</t>
+  </si>
+  <si>
+    <t>coef4_interactive</t>
+  </si>
+  <si>
+    <t>coef5_interactive</t>
+  </si>
+  <si>
     <t>sd1_interactive</t>
   </si>
   <si>
     <t>sd2_interactive</t>
+  </si>
+  <si>
+    <t>sd3_interactive</t>
+  </si>
+  <si>
+    <t>sd4_interactive</t>
+  </si>
+  <si>
+    <t>sd5_interactive</t>
   </si>
   <si>
     <t>1</t>
@@ -193,22 +205,22 @@
       <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="U1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="V1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W1" t="e">
-        <v>#N/A</v>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
         <v>100.0</v>
@@ -279,7 +291,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3" t="e">
         <v>#N/A</v>
@@ -350,7 +362,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" t="e">
         <v>#N/A</v>
@@ -421,7 +433,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" t="e">
         <v>#N/A</v>
@@ -492,7 +504,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B6" t="e">
         <v>#N/A</v>
@@ -563,7 +575,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" t="e">
         <v>#N/A</v>
@@ -634,7 +646,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" t="e">
         <v>#N/A</v>

</xml_diff>